<commit_message>
import data almost done
</commit_message>
<xml_diff>
--- a/test/1. 各院彙整資料/政治大學.xlsx
+++ b/test/1. 各院彙整資料/政治大學.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\3. Index-Evaluation-Analysis-Report\test\1. 各院彙整資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819D227D-0BEE-4E44-9E2D-34DE32A4A414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3149ED1-4DCE-4843-A6E9-23255F9790AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="600" windowWidth="17595" windowHeight="15600" firstSheet="4" activeTab="7" xr2:uid="{5637C56F-4A66-4FBD-9450-EB78733DF21C}"/>
+    <workbookView xWindow="2730" yWindow="600" windowWidth="17595" windowHeight="15600" firstSheet="6" activeTab="7" xr2:uid="{5637C56F-4A66-4FBD-9450-EB78733DF21C}"/>
   </bookViews>
   <sheets>
     <sheet name="小結" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
     <sheet name="2.3.1.2 各系所教師兼任本校二級學術行政主管人次" sheetId="14" r:id="rId7"/>
     <sheet name="3.2.1.1 舉辦國際學術研討會數" sheetId="15" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.1.1.1 學士班繁星推薦入學錄取率'!$A$1:$G$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1.1.3.4 博士班招收國內重點大學畢業生比率'!$A$1:$G$13</definedName>
@@ -53,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="42">
   <si>
     <t>全校</t>
   </si>
@@ -147,45 +144,59 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>100 文學院</t>
-  </si>
-  <si>
-    <t>700 理學院</t>
-  </si>
-  <si>
-    <t>200 社會科學學院</t>
-  </si>
-  <si>
-    <t>600 法學院</t>
-  </si>
-  <si>
-    <t>300 商學院</t>
-  </si>
-  <si>
-    <t>500 外國語文學院</t>
-  </si>
-  <si>
-    <t>400 傳播學院</t>
-  </si>
-  <si>
-    <t>800 國際事務學院</t>
-  </si>
-  <si>
-    <t>900 教育學院</t>
-  </si>
-  <si>
-    <t>Z23 創新國際學院</t>
-  </si>
-  <si>
-    <t>ZA0 資訊學院</t>
-  </si>
-  <si>
     <t>資</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>校加總</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 文學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>700 理學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200 社會科學學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600 法學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300 商學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>500 外國語文學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400 傳播學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>800 國際事務學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>900 教育學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z23 創新國際學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZA0 資訊學院（院加總 / 院均值）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -549,10 +560,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.1061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2069</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1268</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,10 +684,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>9.3600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4399999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5099999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23230000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7599999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,10 +808,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>8.8200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2900000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6499999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6100000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.04</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,10 +1080,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>9.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4800000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13689999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.91E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.05</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,10 +1451,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.1061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2069</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1268</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,10 +1575,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>9.3600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4399999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5099999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23230000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7599999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,10 +1699,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>8.8200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2900000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6499999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6100000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.04</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1750,10 +1971,40 @@
                 <c:formatCode>0.00%;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>9.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4800000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13689999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.91E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.05</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2091,10 +2342,40 @@
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.1061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2069</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1268</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2185,10 +2466,40 @@
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>9.3600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4399999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5099999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23230000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7599999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2279,10 +2590,40 @@
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>8.8200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2900000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6499999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6100000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.04</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2521,10 +2862,40 @@
                 <c:formatCode>#,##0;"—";"—"</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.06</c:v>
+                  <c:v>9.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4800000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13689999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.91E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.89E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.05</c:v>
+                  <c:v>7.8700000000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6066,72 +6437,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="主控台"/>
-      <sheetName val="template"/>
-      <sheetName val="test1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>三年均值</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>110年</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>109年</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>108年</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>科系1</v>
-          </cell>
-          <cell r="C2">
-            <v>0.06</v>
-          </cell>
-          <cell r="D2">
-            <v>0.06</v>
-          </cell>
-          <cell r="E2">
-            <v>0.03</v>
-          </cell>
-          <cell r="F2">
-            <v>1.4999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>院均值</v>
-          </cell>
-          <cell r="C3">
-            <v>0.05</v>
-          </cell>
-          <cell r="D3">
-            <v>0.04</v>
-          </cell>
-          <cell r="E3">
-            <v>0.01</v>
-          </cell>
-          <cell r="F3">
-            <v>3.5000000000000003E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
@@ -6536,7 +6841,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6580,170 +6885,272 @@
         <v>27</v>
       </c>
       <c r="C2" s="10">
-        <v>0.06</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="D2" s="10">
-        <v>0.06</v>
+        <v>8.8200000000000001E-2</v>
       </c>
       <c r="E2" s="10">
-        <v>0.03</v>
+        <v>9.3600000000000003E-2</v>
       </c>
       <c r="F2" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G2" s="9"/>
+        <v>0.1061</v>
+      </c>
+      <c r="G2" s="9">
+        <v>998</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="10">
+        <v>0.1162</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.1018</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.1235</v>
+      </c>
+      <c r="G3" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="10">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.1633</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.2069</v>
+      </c>
+      <c r="G4" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="10">
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="10">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="10">
+        <v>0.1109</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="E7" s="10">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.1615</v>
+      </c>
+      <c r="G7" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="10">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="E8" s="10">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="10">
+        <v>0.1134</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8.6499999999999994E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.1429</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.1268</v>
+      </c>
+      <c r="G10" s="9">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="10">
+        <v>5.91E-2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="E11" s="10">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="F11" s="10">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="10">
+        <v>1.89E-2</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.89E-2</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="10">
-        <v>0.05</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="D13" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F13" s="10">
-        <v>3.5000000000000003E-2</v>
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="G13" s="9">
-        <v>999</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6765,7 +7172,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6809,170 +7216,272 @@
         <v>27</v>
       </c>
       <c r="C2" s="10">
-        <v>0.06</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="D2" s="10">
-        <v>0.06</v>
+        <v>8.8200000000000001E-2</v>
       </c>
       <c r="E2" s="10">
-        <v>0.03</v>
+        <v>9.3600000000000003E-2</v>
       </c>
       <c r="F2" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G2" s="9"/>
+        <v>0.1061</v>
+      </c>
+      <c r="G2" s="9">
+        <v>998</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="10">
+        <v>0.1162</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.1018</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.1235</v>
+      </c>
+      <c r="G3" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="10">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.1633</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.2069</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="10">
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="10">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="10">
+        <v>0.1109</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="E7" s="10">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.1615</v>
+      </c>
+      <c r="G7" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="10">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="E8" s="10">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="10">
+        <v>0.1134</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8.6499999999999994E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.1429</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.1268</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="10">
+        <v>5.91E-2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="E11" s="10">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="F11" s="10">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="10">
+        <v>1.89E-2</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.89E-2</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="10">
-        <v>0.05</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="D13" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F13" s="10">
-        <v>3.5000000000000003E-2</v>
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="G13" s="9">
-        <v>999</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6994,7 +7503,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7038,170 +7547,272 @@
         <v>27</v>
       </c>
       <c r="C2" s="11">
-        <v>0.06</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="D2" s="11">
-        <v>0.06</v>
+        <v>8.8200000000000001E-2</v>
       </c>
       <c r="E2" s="11">
-        <v>0.03</v>
+        <v>9.3600000000000003E-2</v>
       </c>
       <c r="F2" s="11">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G2" s="9"/>
+        <v>0.1061</v>
+      </c>
+      <c r="G2" s="9">
+        <v>998</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="11">
+        <v>0.1162</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.1018</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.1235</v>
+      </c>
+      <c r="G3" s="9">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="11">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.1633</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.2069</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="11">
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="D5" s="11">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="F5" s="11">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="11">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.14549999999999999</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="9"/>
+      <c r="C7" s="11">
+        <v>0.1109</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="E7" s="11">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.1615</v>
+      </c>
+      <c r="G7" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="11">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="D8" s="11">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F8" s="11">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="11">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="11">
+        <v>0.1134</v>
+      </c>
+      <c r="D10" s="11">
+        <v>8.6499999999999994E-2</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.1429</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.1268</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="11">
+        <v>5.91E-2</v>
+      </c>
+      <c r="D11" s="11">
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="E11" s="11">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="F11" s="11">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="11">
+        <v>1.89E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1.89E-2</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="11">
-        <v>0.05</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="D13" s="11">
-        <v>0.04</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="F13" s="11">
-        <v>3.5000000000000003E-2</v>
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="G13" s="9">
-        <v>999</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7223,7 +7834,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7282,7 +7893,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -7295,7 +7906,7 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -7308,7 +7919,7 @@
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -7321,7 +7932,7 @@
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -7334,7 +7945,7 @@
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -7347,7 +7958,7 @@
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -7360,7 +7971,7 @@
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -7373,7 +7984,7 @@
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
@@ -7386,7 +7997,7 @@
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -7399,7 +8010,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -7412,10 +8023,10 @@
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="12">
         <v>0.05</v>
@@ -7452,7 +8063,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7511,7 +8122,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -7524,7 +8135,7 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -7537,7 +8148,7 @@
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -7550,7 +8161,7 @@
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -7563,7 +8174,7 @@
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -7576,7 +8187,7 @@
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -7589,7 +8200,7 @@
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -7602,7 +8213,7 @@
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
@@ -7615,7 +8226,7 @@
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -7628,7 +8239,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -7641,10 +8252,10 @@
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="12">
         <v>0.05</v>
@@ -7681,7 +8292,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7722,7 +8333,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C2" s="12">
         <v>0.06</v>
@@ -7740,7 +8351,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -7753,7 +8364,7 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -7766,7 +8377,7 @@
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -7779,7 +8390,7 @@
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -7792,7 +8403,7 @@
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -7805,7 +8416,7 @@
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -7818,7 +8429,7 @@
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -7831,7 +8442,7 @@
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
@@ -7844,7 +8455,7 @@
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -7857,7 +8468,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -7870,10 +8481,10 @@
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="12">
         <v>0.05</v>
@@ -7910,7 +8521,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7951,7 +8562,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C2" s="12">
         <v>0.06</v>
@@ -7969,7 +8580,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -7982,7 +8593,7 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>2</v>
@@ -7995,7 +8606,7 @@
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -8008,7 +8619,7 @@
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -8021,7 +8632,7 @@
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -8034,7 +8645,7 @@
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -8047,7 +8658,7 @@
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -8060,7 +8671,7 @@
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>8</v>
@@ -8073,7 +8684,7 @@
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>9</v>
@@ -8086,7 +8697,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -8099,10 +8710,10 @@
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C13" s="12">
         <v>0.05</v>

</xml_diff>